<commit_message>
four func run together
</commit_message>
<xml_diff>
--- a/tmp/temp.xlsx
+++ b/tmp/temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYZ_folder\ChallengeCup-Excelerate\A_have_ignored_\Excelerate_backend_original_code\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{797024A8-EDE9-4864-A58D-3F457FBD2603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7220879-3E1F-4C62-B3DE-E0FF068CA52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="2990" windowWidth="10800" windowHeight="7810"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>请以学院为单位汇总完成此Excel后提交至pku62747382@163.com；文件命名方式：五四青年科学奖+院系名称</t>
   </si>
@@ -92,24 +92,6 @@
   </si>
   <si>
     <t>指导教师电子邮箱</t>
-  </si>
-  <si>
-    <t>五四青年科学奖</t>
-  </si>
-  <si>
-    <t>历史学</t>
-  </si>
-  <si>
-    <t>注：</t>
-  </si>
-  <si>
-    <t>1. 每份作品需用粗外侧框线框进行标记；</t>
-  </si>
-  <si>
-    <t>2. 如有多名作者则所有作者信息都需填写；</t>
-  </si>
-  <si>
-    <t>3. 出生年月格式（例）：1999.02。</t>
   </si>
 </sst>
 </file>
@@ -128,7 +110,6 @@
       <sz val="9"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -431,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -583,46 +564,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="6" spans="1:22" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:22" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:22" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:22" ht="14" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:V2"/>

</xml_diff>